<commit_message>
Pemeriksaan Pemantauan Dinamis Multiple Unstable Object Fixing
</commit_message>
<xml_diff>
--- a/Pemadanan Data.xlsx
+++ b/Pemadanan Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BillyBu\Katalon Studio\Awasrik BPJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4CBD2F-2E04-42A5-8AD3-16091A84AD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7E35DE-8F14-4FFB-BA36-88934C7B65CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="15972" windowHeight="10764" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
   </bookViews>
   <sheets>
     <sheet name="inquiry" sheetId="1" r:id="rId1"/>
@@ -72,10 +72,10 @@
     <t>2715000</t>
   </si>
   <si>
-    <t>01732701</t>
-  </si>
-  <si>
     <t>0173</t>
+  </si>
+  <si>
+    <t>01732290</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,10 +644,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Take out robot jadi switch to window. coba tc negative
</commit_message>
<xml_diff>
--- a/Pemadanan Data.xlsx
+++ b/Pemadanan Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BillyBu\Katalon Studio\Awasrik BPJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7E35DE-8F14-4FFB-BA36-88934C7B65CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9F997C-C60B-4F49-8966-25B0B204FFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="15972" windowHeight="10764" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
+    <workbookView xWindow="6504" yWindow="1284" windowWidth="15972" windowHeight="10764" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
   </bookViews>
   <sheets>
     <sheet name="inquiry" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>0173</t>
   </si>
   <si>
-    <t>01732290</t>
+    <t>01732299</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
delete container, fixing screenshot pdf
</commit_message>
<xml_diff>
--- a/Pemadanan Data.xlsx
+++ b/Pemadanan Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BillyBu\Katalon Studio\Awasrik BPJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9F997C-C60B-4F49-8966-25B0B204FFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B58012-963A-47E8-ABE5-2EA4AE0672CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6504" yWindow="1284" windowWidth="15972" windowHeight="10764" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
   </bookViews>
   <sheets>
     <sheet name="inquiry" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>0173</t>
   </si>
   <si>
-    <t>01732299</t>
+    <t>01732301</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
push incrementing global varialbe
</commit_message>
<xml_diff>
--- a/Pemadanan Data.xlsx
+++ b/Pemadanan Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BillyBu\Katalon Studio\Awasrik BPJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B58012-963A-47E8-ABE5-2EA4AE0672CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53EC2BB-F166-437D-967A-EA15C4D4B249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
+    <workbookView xWindow="6504" yWindow="1284" windowWidth="15972" windowHeight="10764" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
   </bookViews>
   <sheets>
     <sheet name="inquiry" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>0173</t>
   </si>
   <si>
-    <t>01732301</t>
+    <t>01732304</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Push Test Suite Negative
</commit_message>
<xml_diff>
--- a/Pemadanan Data.xlsx
+++ b/Pemadanan Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BillyBu\Katalon Studio\Awasrik BPJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53EC2BB-F166-437D-967A-EA15C4D4B249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2158173-6DEB-47C2-BF20-0FFD1722A517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6504" yWindow="1284" windowWidth="15972" windowHeight="10764" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
   </bookViews>
   <sheets>
     <sheet name="inquiry" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>0173</t>
   </si>
   <si>
-    <t>01732304</t>
+    <t>01732306</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Update Listener for all Suite to call KodeBU global
</commit_message>
<xml_diff>
--- a/Pemadanan Data.xlsx
+++ b/Pemadanan Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BillyBu\Katalon Studio\Awasrik BPJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2158173-6DEB-47C2-BF20-0FFD1722A517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B806E83-47B5-4412-B004-C66016F4CE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
+    <workbookView xWindow="1536" yWindow="96" windowWidth="19548" windowHeight="10764" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
   </bookViews>
   <sheets>
     <sheet name="inquiry" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>0173</t>
   </si>
   <si>
-    <t>01732306</t>
+    <t>01730306</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Validation for dynamic cell for TC Sanksi button next page
</commit_message>
<xml_diff>
--- a/Pemadanan Data.xlsx
+++ b/Pemadanan Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BillyBu\Katalon Studio\Awasrik BPJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B806E83-47B5-4412-B004-C66016F4CE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DC1782-D9D5-4672-A1BB-F8FD5F4FB344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="96" windowWidth="19548" windowHeight="10764" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
+    <workbookView xWindow="2232" yWindow="792" windowWidth="19548" windowHeight="10764" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
   </bookViews>
   <sheets>
     <sheet name="inquiry" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>0173</t>
   </si>
   <si>
-    <t>01730306</t>
+    <t>01733707</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fixing tc sanksi cell data validation dynamic remove element present
</commit_message>
<xml_diff>
--- a/Pemadanan Data.xlsx
+++ b/Pemadanan Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BillyBu\Katalon Studio\Awasrik BPJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DC1782-D9D5-4672-A1BB-F8FD5F4FB344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8073BE-2DDF-45B0-8929-FAB364C3EF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2232" yWindow="792" windowWidth="19548" windowHeight="10764" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>0173</t>
   </si>
   <si>
-    <t>01733707</t>
+    <t>01733709</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
update dynamic excel keyword
</commit_message>
<xml_diff>
--- a/Pemadanan Data.xlsx
+++ b/Pemadanan Data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BillyBu\Katalon Studio\Awasrik BPJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8073BE-2DDF-45B0-8929-FAB364C3EF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{07496F57-BE1F-441D-891D-8495FDDB2608}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="792" windowWidth="19548" windowHeight="10764" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}"/>
+    <workbookView windowHeight="10764" windowWidth="19548" xWindow="2580" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}" yWindow="1140"/>
   </bookViews>
   <sheets>
-    <sheet name="inquiry" sheetId="1" r:id="rId1"/>
+    <sheet name="inquiry" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>NPP</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>01733709</t>
+  </si>
+  <si>
+    <t>01733710</t>
   </si>
 </sst>
 </file>
@@ -204,36 +207,36 @@
     </border>
   </borders>
   <cellStyleXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="41"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="8" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" quotePrefix="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma [0] 2" xfId="1" xr:uid="{1CD0CB7D-E524-4377-BE5D-5C3AA6932F70}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="6" xr:uid="{59DA184D-F75B-4F39-A6A6-83A5ECA80886}"/>
     <cellStyle name="Normal 2 2" xfId="3" xr:uid="{4C12C8E8-4646-4CF1-BAB5-B4F50443B786}"/>
     <cellStyle name="Normal 27" xfId="2" xr:uid="{27E575A1-51FA-4490-AB14-D2D82298062D}"/>
@@ -272,7 +275,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -289,10 +292,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -327,7 +330,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -379,7 +382,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -490,21 +493,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -521,7 +524,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -593,15 +596,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FE76B6-18FB-4525-B864-3FE4BB25A71D}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FE76B6-18FB-4525-B864-3FE4BB25A71D}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -609,14 +612,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="28.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="21" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="12.5546875" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="14.33203125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="4" width="14.44140625" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="4" width="28.44140625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="17.21875" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="4" width="21.44140625" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="4" width="21.0" collapsed="false"/>
+    <col min="8" max="16384" style="4" width="9.109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -644,7 +647,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>12</v>
@@ -668,12 +671,12 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="E2">
-    <cfRule type="duplicateValues" dxfId="2" priority="10"/>
+    <cfRule dxfId="2" priority="10" type="duplicateValues"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="duplicateValues" dxfId="1" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
+    <cfRule dxfId="1" priority="11" type="duplicateValues"/>
+    <cfRule dxfId="0" priority="12" type="duplicateValues"/>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Coordination Test data Keyword and Listener, add Dynamic Date for TC Sanksi
</commit_message>
<xml_diff>
--- a/Pemadanan Data.xlsx
+++ b/Pemadanan Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BillyBu\Katalon Studio\Awasrik BPJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{07496F57-BE1F-441D-891D-8495FDDB2608}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{2E24EE16-3579-4F62-BA46-04F9701BC886}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="10764" windowWidth="19548" xWindow="2580" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}" yWindow="1140"/>
+    <workbookView windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{03A78402-4A73-411C-800E-A848D3077229}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="inquiry" r:id="rId1" sheetId="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>NPP</t>
   </si>
@@ -75,10 +75,13 @@
     <t>0173</t>
   </si>
   <si>
-    <t>01733709</t>
-  </si>
-  <si>
-    <t>01733710</t>
+    <t>01733720</t>
+  </si>
+  <si>
+    <t>01733721</t>
+  </si>
+  <si>
+    <t>01733722</t>
   </si>
 </sst>
 </file>
@@ -612,14 +615,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="12.5546875" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="14.33203125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="4" width="14.44140625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="4" width="28.44140625" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="17.21875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="4" width="21.44140625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="4" width="21.0" collapsed="false"/>
-    <col min="8" max="16384" style="4" width="9.109375" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="12.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="14.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="14.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="28.44140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="17.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="21.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="21.0" collapsed="true"/>
+    <col min="8" max="16384" style="4" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -647,7 +650,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
push dynamic sanksi with multiple table page
</commit_message>
<xml_diff>
--- a/Pemadanan Data.xlsx
+++ b/Pemadanan Data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>NPP</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>01733722</t>
+  </si>
+  <si>
+    <t>01733723</t>
+  </si>
+  <si>
+    <t>01733724</t>
+  </si>
+  <si>
+    <t>01733725</t>
   </si>
 </sst>
 </file>
@@ -650,7 +659,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>12</v>

</xml_diff>